<commit_message>
Update Des Scheduled Flights vs actual.xlsx
</commit_message>
<xml_diff>
--- a/codeLibrary/R/R/airlineData/Des Scheduled Flights vs actual.xlsx
+++ b/codeLibrary/R/R/airlineData/Des Scheduled Flights vs actual.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cjseeger/Sites/LVM-Code/codeLibrary/R/R/airlineData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C294ED02-B74B-E041-81E2-3C4A56461EB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFFFE7E-C19B-0045-9AA4-F410B82073E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="3360" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="151">
   <si>
     <t>Chart</t>
   </si>
@@ -441,6 +441,48 @@
   </si>
   <si>
     <t>2020-08-18</t>
+  </si>
+  <si>
+    <t>2020-08-19</t>
+  </si>
+  <si>
+    <t>2020-08-20</t>
+  </si>
+  <si>
+    <t>2020-08-21</t>
+  </si>
+  <si>
+    <t>2020-08-22</t>
+  </si>
+  <si>
+    <t>2020-08-23</t>
+  </si>
+  <si>
+    <t>2020-08-24</t>
+  </si>
+  <si>
+    <t>2020-08-25</t>
+  </si>
+  <si>
+    <t>2020-08-26</t>
+  </si>
+  <si>
+    <t>2020-08-27</t>
+  </si>
+  <si>
+    <t>2020-08-28</t>
+  </si>
+  <si>
+    <t>2020-08-29</t>
+  </si>
+  <si>
+    <t>2020-08-30</t>
+  </si>
+  <si>
+    <t>2020-08-31</t>
+  </si>
+  <si>
+    <t>2020-09-01</t>
   </si>
 </sst>
 </file>
@@ -1312,10 +1354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D135"/>
+  <dimension ref="A1:D149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="F134" sqref="F134"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="G144" sqref="G144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
@@ -3306,7 +3348,7 @@
         <v>53</v>
       </c>
       <c r="D133" s="3">
-        <f t="shared" ref="D133:D135" si="2">C133/B133</f>
+        <f t="shared" ref="D133:D149" si="2">C133/B133</f>
         <v>0.92982456140350878</v>
       </c>
     </row>
@@ -3338,6 +3380,216 @@
       <c r="D135" s="3">
         <f t="shared" si="2"/>
         <v>0.95833333333333337</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="A136" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B136" s="2">
+        <v>50</v>
+      </c>
+      <c r="C136" s="2">
+        <v>48</v>
+      </c>
+      <c r="D136" s="3">
+        <f t="shared" si="2"/>
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="A137" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B137" s="2">
+        <v>52</v>
+      </c>
+      <c r="C137" s="2">
+        <v>48</v>
+      </c>
+      <c r="D137" s="3">
+        <f t="shared" si="2"/>
+        <v>0.92307692307692313</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B138" s="2">
+        <v>58</v>
+      </c>
+      <c r="C138" s="2">
+        <v>52</v>
+      </c>
+      <c r="D138" s="3">
+        <f t="shared" si="2"/>
+        <v>0.89655172413793105</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="A139" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B139" s="2">
+        <v>51</v>
+      </c>
+      <c r="C139" s="2">
+        <v>48</v>
+      </c>
+      <c r="D139" s="3">
+        <f t="shared" si="2"/>
+        <v>0.94117647058823528</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
+      <c r="A140" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B140" s="2">
+        <v>48</v>
+      </c>
+      <c r="C140" s="2">
+        <v>44</v>
+      </c>
+      <c r="D140" s="3">
+        <f t="shared" si="2"/>
+        <v>0.91666666666666663</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
+      <c r="A141" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B141" s="2">
+        <v>56</v>
+      </c>
+      <c r="C141" s="2">
+        <v>52</v>
+      </c>
+      <c r="D141" s="3">
+        <f t="shared" si="2"/>
+        <v>0.9285714285714286</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4">
+      <c r="A142" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B142" s="2">
+        <v>45</v>
+      </c>
+      <c r="C142" s="2">
+        <v>42</v>
+      </c>
+      <c r="D142" s="3">
+        <f t="shared" si="2"/>
+        <v>0.93333333333333335</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4">
+      <c r="A143" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B143" s="2">
+        <v>52</v>
+      </c>
+      <c r="C143" s="2">
+        <v>46</v>
+      </c>
+      <c r="D143" s="3">
+        <f t="shared" si="2"/>
+        <v>0.88461538461538458</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
+      <c r="A144" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B144" s="2">
+        <v>71</v>
+      </c>
+      <c r="C144" s="2">
+        <v>64</v>
+      </c>
+      <c r="D144" s="3">
+        <f t="shared" si="2"/>
+        <v>0.90140845070422537</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
+      <c r="A145" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B145" s="2">
+        <v>55</v>
+      </c>
+      <c r="C145" s="2">
+        <v>50</v>
+      </c>
+      <c r="D145" s="3">
+        <f t="shared" si="2"/>
+        <v>0.90909090909090906</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
+      <c r="A146" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B146" s="2">
+        <v>46</v>
+      </c>
+      <c r="C146" s="2">
+        <v>43</v>
+      </c>
+      <c r="D146" s="3">
+        <f t="shared" si="2"/>
+        <v>0.93478260869565222</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
+      <c r="A147" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B147" s="2">
+        <v>51</v>
+      </c>
+      <c r="C147" s="2">
+        <v>46</v>
+      </c>
+      <c r="D147" s="3">
+        <f t="shared" si="2"/>
+        <v>0.90196078431372551</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4">
+      <c r="A148" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B148" s="2">
+        <v>52</v>
+      </c>
+      <c r="C148" s="2">
+        <v>49</v>
+      </c>
+      <c r="D148" s="3">
+        <f t="shared" si="2"/>
+        <v>0.94230769230769229</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
+      <c r="A149" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B149" s="2">
+        <v>45</v>
+      </c>
+      <c r="C149" s="2">
+        <v>44</v>
+      </c>
+      <c r="D149" s="3">
+        <f t="shared" si="2"/>
+        <v>0.97777777777777775</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to airline data
</commit_message>
<xml_diff>
--- a/codeLibrary/R/R/airlineData/Des Scheduled Flights vs actual.xlsx
+++ b/codeLibrary/R/R/airlineData/Des Scheduled Flights vs actual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cjseeger/Sites/LVM-Code/codeLibrary/R/R/airlineData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB40B12-EE98-A64D-A5D6-D6A61231FA8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7108397B-D5BF-8A4F-A23B-BC94BE0F2940}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2360" yWindow="2140" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="291">
   <si>
     <t>Chart</t>
   </si>
@@ -849,6 +849,60 @@
   </si>
   <si>
     <t>2021-01-01</t>
+  </si>
+  <si>
+    <t>2021-01-02</t>
+  </si>
+  <si>
+    <t>2021-01-03</t>
+  </si>
+  <si>
+    <t>2021-01-04</t>
+  </si>
+  <si>
+    <t>2021-01-05</t>
+  </si>
+  <si>
+    <t>2021-01-06</t>
+  </si>
+  <si>
+    <t>2021-01-07</t>
+  </si>
+  <si>
+    <t>2021-01-08</t>
+  </si>
+  <si>
+    <t>2021-01-09</t>
+  </si>
+  <si>
+    <t>2021-01-10</t>
+  </si>
+  <si>
+    <t>2021-01-11</t>
+  </si>
+  <si>
+    <t>2021-01-12</t>
+  </si>
+  <si>
+    <t>2021-01-13</t>
+  </si>
+  <si>
+    <t>2021-01-14</t>
+  </si>
+  <si>
+    <t>2021-01-15</t>
+  </si>
+  <si>
+    <t>2021-01-16</t>
+  </si>
+  <si>
+    <t>2021-01-17</t>
+  </si>
+  <si>
+    <t>2021-01-18</t>
+  </si>
+  <si>
+    <t>2021-01-19</t>
   </si>
 </sst>
 </file>
@@ -1720,10 +1774,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D271"/>
+  <dimension ref="A1:D289"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A236" workbookViewId="0">
-      <selection activeCell="G270" sqref="G269:G270"/>
+    <sheetView tabSelected="1" topLeftCell="A278" workbookViewId="0">
+      <selection activeCell="I279" sqref="I279"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5634,7 +5688,7 @@
         <v>55</v>
       </c>
       <c r="D261" s="3">
-        <f t="shared" ref="D261:D271" si="4">C261/B261</f>
+        <f t="shared" ref="D261:D289" si="4">C261/B261</f>
         <v>1</v>
       </c>
     </row>
@@ -5786,6 +5840,276 @@
       <c r="D271" s="3">
         <f t="shared" si="4"/>
         <v>0.91176470588235292</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A272" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B272" s="2">
+        <v>57</v>
+      </c>
+      <c r="C272" s="2">
+        <v>54</v>
+      </c>
+      <c r="D272" s="3">
+        <f t="shared" si="4"/>
+        <v>0.94736842105263153</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A273" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="B273" s="2">
+        <v>52</v>
+      </c>
+      <c r="C273" s="2">
+        <v>50</v>
+      </c>
+      <c r="D273" s="3">
+        <f t="shared" si="4"/>
+        <v>0.96153846153846156</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A274" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B274" s="2">
+        <v>55</v>
+      </c>
+      <c r="C274" s="2">
+        <v>49</v>
+      </c>
+      <c r="D274" s="3">
+        <f t="shared" si="4"/>
+        <v>0.89090909090909087</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A275" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B275" s="2">
+        <v>45</v>
+      </c>
+      <c r="C275" s="2">
+        <v>43</v>
+      </c>
+      <c r="D275" s="3">
+        <f t="shared" si="4"/>
+        <v>0.9555555555555556</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A276" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B276" s="2">
+        <v>41</v>
+      </c>
+      <c r="C276" s="2">
+        <v>40</v>
+      </c>
+      <c r="D276" s="3">
+        <f t="shared" si="4"/>
+        <v>0.97560975609756095</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A277" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B277" s="2">
+        <v>53</v>
+      </c>
+      <c r="C277" s="2">
+        <v>50</v>
+      </c>
+      <c r="D277" s="3">
+        <f t="shared" si="4"/>
+        <v>0.94339622641509435</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A278" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B278" s="2">
+        <v>48</v>
+      </c>
+      <c r="C278" s="2">
+        <v>47</v>
+      </c>
+      <c r="D278" s="3">
+        <f t="shared" si="4"/>
+        <v>0.97916666666666663</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A279" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B279" s="2">
+        <v>42</v>
+      </c>
+      <c r="C279" s="2">
+        <v>41</v>
+      </c>
+      <c r="D279" s="3">
+        <f t="shared" si="4"/>
+        <v>0.97619047619047616</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A280" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="B280" s="2">
+        <v>48</v>
+      </c>
+      <c r="C280" s="2">
+        <v>46</v>
+      </c>
+      <c r="D280" s="3">
+        <f t="shared" si="4"/>
+        <v>0.95833333333333337</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A281" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B281" s="2">
+        <v>39</v>
+      </c>
+      <c r="C281" s="2">
+        <v>37</v>
+      </c>
+      <c r="D281" s="3">
+        <f t="shared" si="4"/>
+        <v>0.94871794871794868</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A282" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B282" s="2">
+        <v>49</v>
+      </c>
+      <c r="C282" s="2">
+        <v>47</v>
+      </c>
+      <c r="D282" s="3">
+        <f t="shared" si="4"/>
+        <v>0.95918367346938771</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A283" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B283" s="2">
+        <v>47</v>
+      </c>
+      <c r="C283" s="2">
+        <v>45</v>
+      </c>
+      <c r="D283" s="3">
+        <f t="shared" si="4"/>
+        <v>0.95744680851063835</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A284" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B284" s="2">
+        <v>48</v>
+      </c>
+      <c r="C284" s="2">
+        <v>48</v>
+      </c>
+      <c r="D284" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A285" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B285" s="2">
+        <v>38</v>
+      </c>
+      <c r="C285" s="2">
+        <v>38</v>
+      </c>
+      <c r="D285" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A286" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B286" s="2">
+        <v>47</v>
+      </c>
+      <c r="C286" s="2">
+        <v>46</v>
+      </c>
+      <c r="D286" s="3">
+        <f t="shared" si="4"/>
+        <v>0.97872340425531912</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A287" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B287" s="2">
+        <v>36</v>
+      </c>
+      <c r="C287" s="2">
+        <v>36</v>
+      </c>
+      <c r="D287" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A288" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B288" s="2">
+        <v>44</v>
+      </c>
+      <c r="C288" s="2">
+        <v>43</v>
+      </c>
+      <c r="D288" s="3">
+        <f t="shared" si="4"/>
+        <v>0.97727272727272729</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A289" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B289" s="2">
+        <v>41</v>
+      </c>
+      <c r="C289" s="2">
+        <v>37</v>
+      </c>
+      <c r="D289" s="3">
+        <f t="shared" si="4"/>
+        <v>0.90243902439024393</v>
       </c>
     </row>
   </sheetData>

</xml_diff>